<commit_message>
Removed unnecessary usings and tested excel
</commit_message>
<xml_diff>
--- a/SharedFiles/Contacts.xlsx
+++ b/SharedFiles/Contacts.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>FullName</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>asd</t>
+  </si>
+  <si>
+    <t>Андрей Андреев</t>
+  </si>
+  <si>
+    <t>andreyandreev@mail.ru</t>
+  </si>
+  <si>
+    <t>+380957894561</t>
   </si>
 </sst>
 </file>
@@ -144,7 +153,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -250,6 +259,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Added error page and correct routing at navbar
</commit_message>
<xml_diff>
--- a/SharedFiles/Contacts.xlsx
+++ b/SharedFiles/Contacts.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>FullName</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>+380957894561</t>
+  </si>
+  <si>
+    <t>Максим Шило</t>
+  </si>
+  <si>
+    <t>mamkotraxer@gmail.com</t>
+  </si>
+  <si>
+    <t>Mamu ebal</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -276,6 +285,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>